<commit_message>
DataFrame was corrected, cours_pass series was added.
</commit_message>
<xml_diff>
--- a/Lesson_32/students.xlsx
+++ b/Lesson_32/students.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Game On Dp\PycharmProjects\PDS\Lesson_32\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA8CCDAB-7BB3-458D-A466-09A193DD1E9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5E4B865-45AA-4A2A-B79F-6356403C46BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>name</t>
   </si>
@@ -91,6 +91,9 @@
   </si>
   <si>
     <t>John</t>
+  </si>
+  <si>
+    <t>course_pass</t>
   </si>
 </sst>
 </file>
@@ -418,19 +421,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="11" customWidth="1"/>
     <col min="3" max="3" width="10.7109375" customWidth="1"/>
+    <col min="5" max="5" width="12.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -443,14 +447,17 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
       <c r="B2">
         <f ca="1">RANDBETWEEN(C2*8,C2*10)/10</f>
-        <v>9.9</v>
+        <v>8.6999999999999993</v>
       </c>
       <c r="C2">
         <v>10</v>
@@ -459,13 +466,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
       <c r="B3">
         <f t="shared" ref="B3:B16" ca="1" si="0">RANDBETWEEN(C3*8,C3*10)/10</f>
-        <v>6.4</v>
+        <v>7.9</v>
       </c>
       <c r="C3">
         <v>8</v>
@@ -474,13 +481,13 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
       <c r="B4">
         <f t="shared" ca="1" si="0"/>
-        <v>5.8</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="C4">
         <v>6</v>
@@ -489,13 +496,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
       <c r="B5">
         <f t="shared" ca="1" si="0"/>
-        <v>10.7</v>
+        <v>10.9</v>
       </c>
       <c r="C5">
         <v>12</v>
@@ -504,13 +511,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>8</v>
       </c>
       <c r="B6">
         <f t="shared" ca="1" si="0"/>
-        <v>6.7</v>
+        <v>5.6</v>
       </c>
       <c r="C6">
         <v>7</v>
@@ -519,13 +526,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>9</v>
       </c>
       <c r="B7">
         <f t="shared" ca="1" si="0"/>
-        <v>5.8</v>
+        <v>6</v>
       </c>
       <c r="C7">
         <v>6</v>
@@ -534,13 +541,13 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>10</v>
       </c>
       <c r="B8">
         <f t="shared" ca="1" si="0"/>
-        <v>11.1</v>
+        <v>10.6</v>
       </c>
       <c r="C8">
         <v>12</v>
@@ -549,13 +556,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>11</v>
       </c>
       <c r="B9">
         <f t="shared" ca="1" si="0"/>
-        <v>8.9</v>
+        <v>10.7</v>
       </c>
       <c r="C9">
         <v>11</v>
@@ -564,13 +571,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>12</v>
       </c>
       <c r="B10">
         <f t="shared" ca="1" si="0"/>
-        <v>8.8000000000000007</v>
+        <v>9.6999999999999993</v>
       </c>
       <c r="C10">
         <v>10</v>
@@ -579,13 +586,13 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>13</v>
       </c>
       <c r="B11">
         <f t="shared" ca="1" si="0"/>
-        <v>4.4000000000000004</v>
+        <v>4.2</v>
       </c>
       <c r="C11">
         <v>5</v>
@@ -594,13 +601,13 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>14</v>
       </c>
       <c r="B12">
         <f t="shared" ca="1" si="0"/>
-        <v>8</v>
+        <v>8.4</v>
       </c>
       <c r="C12">
         <v>10</v>
@@ -609,13 +616,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>15</v>
       </c>
       <c r="B13">
         <f t="shared" ca="1" si="0"/>
-        <v>10.3</v>
+        <v>11</v>
       </c>
       <c r="C13">
         <v>11</v>
@@ -624,13 +631,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>16</v>
       </c>
       <c r="B14">
         <f t="shared" ca="1" si="0"/>
-        <v>8</v>
+        <v>7.6</v>
       </c>
       <c r="C14">
         <v>9</v>
@@ -639,13 +646,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>17</v>
       </c>
       <c r="B15">
         <f t="shared" ca="1" si="0"/>
-        <v>7.3</v>
+        <v>8.1</v>
       </c>
       <c r="C15">
         <v>9</v>
@@ -654,13 +661,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>18</v>
       </c>
       <c r="B16">
         <f t="shared" ca="1" si="0"/>
-        <v>6.4</v>
+        <v>7.5</v>
       </c>
       <c r="C16">
         <v>8</v>

</xml_diff>